<commit_message>
added lessons to database
</commit_message>
<xml_diff>
--- a/DataBaseExport.xlsx
+++ b/DataBaseExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="19260" windowHeight="7695" tabRatio="811" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="19260" windowHeight="7695" tabRatio="811" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="105">
   <si>
     <t>NULL</t>
   </si>
@@ -286,13 +286,67 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>pol3</t>
+  </si>
+  <si>
+    <t>pol1</t>
+  </si>
+  <si>
+    <t>pol2</t>
+  </si>
+  <si>
+    <t>mat1</t>
+  </si>
+  <si>
+    <t>mat2</t>
+  </si>
+  <si>
+    <t>ma3</t>
+  </si>
+  <si>
+    <t>fiz123</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>re12</t>
+  </si>
+  <si>
+    <t>re23</t>
+  </si>
+  <si>
+    <t>hist123</t>
+  </si>
+  <si>
+    <t>2.1.1.1</t>
+  </si>
+  <si>
+    <t>1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>ang12</t>
+  </si>
+  <si>
+    <t>ang23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,13 +354,45 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -321,12 +407,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -625,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G27" sqref="A10:G27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1510,7 +1618,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D16"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1773,52 +1881,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:U96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="9" style="4"/>
+    <col min="3" max="3" width="9" style="6"/>
+    <col min="4" max="4" width="9" style="8"/>
+    <col min="7" max="7" width="9" style="12"/>
+    <col min="10" max="10" width="3" customWidth="1"/>
+    <col min="11" max="11" width="3.5" customWidth="1"/>
+    <col min="12" max="12" width="4.5" style="8" customWidth="1"/>
+    <col min="13" max="13" width="4.75" customWidth="1"/>
+    <col min="14" max="14" width="3.75" customWidth="1"/>
+    <col min="15" max="15" width="10.875" style="6" customWidth="1"/>
+    <col min="16" max="16" width="4.125" customWidth="1"/>
+    <col min="18" max="18" width="3.375" customWidth="1"/>
+    <col min="19" max="19" width="13.875" style="4" customWidth="1"/>
+    <col min="20" max="20" width="3.75" customWidth="1"/>
+    <col min="21" max="21" width="3.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:21">
       <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2111</v>
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="H1" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="K1" s="1">
+        <v>1</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1">
+        <v>15</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" s="1">
+        <v>1</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="1">
+        <v>1</v>
+      </c>
+      <c r="U1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -1826,157 +1981,3207 @@
       <c r="F2" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>15</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="1">
+        <v>2</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>87</v>
+      </c>
+      <c r="R3" s="1">
+        <v>3</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="L4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4">
+        <v>15</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>90</v>
+      </c>
+      <c r="R4" s="1">
+        <v>4</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="L5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>91</v>
+      </c>
+      <c r="R5" s="1">
+        <v>5</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="L6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>15</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>92</v>
+      </c>
+      <c r="R6" s="1">
+        <v>6</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1">
         <v>4</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
         <v>7</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="L7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7">
+        <v>18</v>
+      </c>
+      <c r="N7">
+        <v>7</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>93</v>
+      </c>
+      <c r="R7" s="1">
+        <v>7</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
         <v>8</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1">
-        <v>1</v>
+      <c r="L8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8">
+        <v>8</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="1">
+        <v>8</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T8" s="1">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>9</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9">
+        <v>9</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="1">
+        <v>9</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T9" s="1">
+        <v>1</v>
+      </c>
+      <c r="U9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>10</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>11</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5">
+        <v>4</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>18</v>
+      </c>
+      <c r="N12">
+        <v>12</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>13</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>14</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>15</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>16</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>6</v>
+      </c>
+      <c r="D18" s="8">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6">
+        <v>7</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6">
+        <v>7</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3</v>
+      </c>
+      <c r="C21" s="6">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
+        <v>3</v>
+      </c>
+      <c r="C22" s="6">
+        <v>7</v>
+      </c>
+      <c r="D22" s="8">
+        <v>4</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3</v>
+      </c>
+      <c r="C23" s="6">
+        <v>7</v>
+      </c>
+      <c r="D23" s="8">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
+        <v>3</v>
+      </c>
+      <c r="C24" s="6">
+        <v>7</v>
+      </c>
+      <c r="D24" s="8">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4">
+        <v>3</v>
+      </c>
+      <c r="C25" s="6">
+        <v>7</v>
+      </c>
+      <c r="D25" s="8">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4">
+        <v>3</v>
+      </c>
+      <c r="C26" s="6">
+        <v>7</v>
+      </c>
+      <c r="D26" s="8">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3</v>
+      </c>
+      <c r="C27" s="6">
+        <v>7</v>
+      </c>
+      <c r="D27" s="8">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4">
+        <v>9</v>
+      </c>
+      <c r="C28" s="6">
+        <v>13</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6">
+        <v>13</v>
+      </c>
+      <c r="D29" s="8">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4">
+        <v>9</v>
+      </c>
+      <c r="C30" s="6">
+        <v>13</v>
+      </c>
+      <c r="D30" s="8">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4">
+        <v>9</v>
+      </c>
+      <c r="C31" s="6">
+        <v>13</v>
+      </c>
+      <c r="D31" s="8">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="4">
+        <v>9</v>
+      </c>
+      <c r="C32" s="6">
+        <v>14</v>
+      </c>
+      <c r="D32" s="8">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4">
+        <v>9</v>
+      </c>
+      <c r="C33" s="6">
+        <v>14</v>
+      </c>
+      <c r="D33" s="8">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4">
+        <v>9</v>
+      </c>
+      <c r="C34" s="6">
+        <v>14</v>
+      </c>
+      <c r="D34" s="8">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="1">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4">
+        <v>9</v>
+      </c>
+      <c r="C35" s="6">
+        <v>14</v>
+      </c>
+      <c r="D35" s="8">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>3</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="1">
+        <v>36</v>
+      </c>
+      <c r="B36" s="4">
+        <v>9</v>
+      </c>
+      <c r="C36" s="6">
+        <v>14</v>
+      </c>
+      <c r="D36" s="8">
+        <v>9</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>3</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" s="1">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6">
+        <v>12</v>
+      </c>
+      <c r="D37" s="8">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>3</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M37">
+        <v>15</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>88</v>
+      </c>
+      <c r="R37" s="1">
+        <v>1</v>
+      </c>
+      <c r="S37" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" s="1">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4">
+        <v>8</v>
+      </c>
+      <c r="C38" s="6">
+        <v>12</v>
+      </c>
+      <c r="D38" s="8">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>3</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>15</v>
+      </c>
+      <c r="N38">
+        <v>2</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>89</v>
+      </c>
+      <c r="R38" s="1">
+        <v>2</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" s="1">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4">
+        <v>8</v>
+      </c>
+      <c r="C39" s="6">
+        <v>12</v>
+      </c>
+      <c r="D39" s="8">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>3</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="K39" s="1">
+        <v>3</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M39">
+        <v>15</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>87</v>
+      </c>
+      <c r="R39" s="1">
+        <v>3</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" s="1">
+        <v>40</v>
+      </c>
+      <c r="B40" s="4">
+        <v>8</v>
+      </c>
+      <c r="C40" s="6">
+        <v>12</v>
+      </c>
+      <c r="D40" s="8">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="K40" s="1">
+        <v>4</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40">
+        <v>15</v>
+      </c>
+      <c r="N40">
+        <v>4</v>
+      </c>
+      <c r="O40" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>90</v>
+      </c>
+      <c r="R40" s="1">
+        <v>4</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" s="1">
+        <v>41</v>
+      </c>
+      <c r="B41" s="4">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6">
+        <v>12</v>
+      </c>
+      <c r="D41" s="8">
+        <v>5</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="K41" s="1">
+        <v>5</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M41">
+        <v>15</v>
+      </c>
+      <c r="N41">
+        <v>5</v>
+      </c>
+      <c r="O41" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>91</v>
+      </c>
+      <c r="R41" s="1">
+        <v>5</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" s="1">
+        <v>42</v>
+      </c>
+      <c r="B42" s="4">
+        <v>8</v>
+      </c>
+      <c r="C42" s="6">
+        <v>12</v>
+      </c>
+      <c r="D42" s="8">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="K42" s="1">
+        <v>6</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M42">
+        <v>15</v>
+      </c>
+      <c r="N42">
+        <v>6</v>
+      </c>
+      <c r="O42" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>92</v>
+      </c>
+      <c r="R42" s="1">
+        <v>6</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="A43" s="1">
+        <v>43</v>
+      </c>
+      <c r="B43" s="4">
+        <v>8</v>
+      </c>
+      <c r="C43" s="6">
+        <v>12</v>
+      </c>
+      <c r="D43" s="8">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1">
+        <v>7</v>
+      </c>
+      <c r="L43" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M43">
+        <v>18</v>
+      </c>
+      <c r="N43">
+        <v>7</v>
+      </c>
+      <c r="O43" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>93</v>
+      </c>
+      <c r="R43" s="1">
+        <v>7</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" s="1">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4">
+        <v>8</v>
+      </c>
+      <c r="C44" s="6">
+        <v>12</v>
+      </c>
+      <c r="D44" s="8">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>3</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1">
+        <v>8</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M44">
+        <v>18</v>
+      </c>
+      <c r="N44">
+        <v>8</v>
+      </c>
+      <c r="O44" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>8</v>
+      </c>
+      <c r="R44" s="1">
+        <v>8</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="A45" s="1">
+        <v>45</v>
+      </c>
+      <c r="B45" s="4">
+        <v>8</v>
+      </c>
+      <c r="C45" s="6">
+        <v>12</v>
+      </c>
+      <c r="D45" s="8">
+        <v>9</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>3</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+      <c r="K45" s="1">
+        <v>9</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M45">
+        <v>18</v>
+      </c>
+      <c r="N45">
+        <v>9</v>
+      </c>
+      <c r="O45" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>8</v>
+      </c>
+      <c r="R45" s="1">
+        <v>9</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" s="1">
+        <v>46</v>
+      </c>
+      <c r="B46" s="4">
+        <v>7</v>
+      </c>
+      <c r="C46" s="6">
+        <v>12</v>
+      </c>
+      <c r="D46" s="8">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>18</v>
+      </c>
+      <c r="N46">
+        <v>10</v>
+      </c>
+      <c r="O46" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="A47" s="1">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4">
+        <v>7</v>
+      </c>
+      <c r="C47" s="6">
+        <v>12</v>
+      </c>
+      <c r="D47" s="8">
+        <v>2</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" s="1">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>11</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" s="1">
+        <v>48</v>
+      </c>
+      <c r="B48" s="4">
+        <v>7</v>
+      </c>
+      <c r="C48" s="6">
+        <v>12</v>
+      </c>
+      <c r="D48" s="8">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H48" s="1">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>18</v>
+      </c>
+      <c r="N48">
+        <v>12</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" s="1">
+        <v>49</v>
+      </c>
+      <c r="B49" s="4">
+        <v>7</v>
+      </c>
+      <c r="C49" s="6">
+        <v>12</v>
+      </c>
+      <c r="D49" s="8">
+        <v>4</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>12</v>
+      </c>
+      <c r="N49">
+        <v>13</v>
+      </c>
+      <c r="O49" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="A50" s="1">
+        <v>50</v>
+      </c>
+      <c r="B50" s="4">
+        <v>7</v>
+      </c>
+      <c r="C50" s="6">
+        <v>12</v>
+      </c>
+      <c r="D50" s="8">
+        <v>5</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>3</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H50" s="1">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>15</v>
+      </c>
+      <c r="N50">
+        <v>14</v>
+      </c>
+      <c r="O50" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="A51" s="1">
+        <v>51</v>
+      </c>
+      <c r="B51" s="4">
+        <v>7</v>
+      </c>
+      <c r="C51" s="6">
+        <v>12</v>
+      </c>
+      <c r="D51" s="13">
+        <v>6</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H51" s="1">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>15</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52" s="1">
+        <v>52</v>
+      </c>
+      <c r="B52" s="4">
+        <v>7</v>
+      </c>
+      <c r="C52" s="6">
+        <v>12</v>
+      </c>
+      <c r="D52" s="13">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>3</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>18</v>
+      </c>
+      <c r="N52">
+        <v>16</v>
+      </c>
+      <c r="O52" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="A53" s="1">
+        <v>53</v>
+      </c>
+      <c r="B53" s="4">
+        <v>7</v>
+      </c>
+      <c r="C53" s="6">
+        <v>12</v>
+      </c>
+      <c r="D53" s="8">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>3</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" s="1">
+        <v>54</v>
+      </c>
+      <c r="B54" s="4">
+        <v>7</v>
+      </c>
+      <c r="C54" s="6">
+        <v>12</v>
+      </c>
+      <c r="D54" s="8">
+        <v>9</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>3</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" s="1">
+        <v>55</v>
+      </c>
+      <c r="B55" s="4">
+        <v>5</v>
+      </c>
+      <c r="C55" s="6">
+        <v>8</v>
+      </c>
+      <c r="D55" s="8">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" s="1">
+        <v>56</v>
+      </c>
+      <c r="B56" s="4">
+        <v>5</v>
+      </c>
+      <c r="C56" s="6">
+        <v>8</v>
+      </c>
+      <c r="D56" s="8">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" s="1">
+        <v>57</v>
+      </c>
+      <c r="B57" s="4">
+        <v>5</v>
+      </c>
+      <c r="C57" s="6">
+        <v>8</v>
+      </c>
+      <c r="D57" s="8">
+        <v>12</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" s="1">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4">
+        <v>5</v>
+      </c>
+      <c r="C58" s="6">
+        <v>8</v>
+      </c>
+      <c r="D58" s="8">
+        <v>13</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="A59" s="1">
+        <v>59</v>
+      </c>
+      <c r="B59" s="4">
+        <v>5</v>
+      </c>
+      <c r="C59" s="6">
+        <v>8</v>
+      </c>
+      <c r="D59" s="8">
+        <v>14</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="A60" s="1">
+        <v>60</v>
+      </c>
+      <c r="B60" s="4">
+        <v>5</v>
+      </c>
+      <c r="C60" s="6">
+        <v>8</v>
+      </c>
+      <c r="D60" s="8">
+        <v>15</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
+      <c r="A61" s="1">
+        <v>61</v>
+      </c>
+      <c r="B61" s="4">
+        <v>5</v>
+      </c>
+      <c r="C61" s="6">
+        <v>10</v>
+      </c>
+      <c r="D61" s="8">
+        <v>16</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="A62" s="1">
+        <v>62</v>
+      </c>
+      <c r="B62" s="4">
+        <v>5</v>
+      </c>
+      <c r="C62" s="6">
+        <v>10</v>
+      </c>
+      <c r="D62" s="8">
+        <v>17</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" s="1">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4">
+        <v>5</v>
+      </c>
+      <c r="C63" s="6">
+        <v>10</v>
+      </c>
+      <c r="D63" s="8">
+        <v>18</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" s="1">
+        <v>64</v>
+      </c>
+      <c r="B64" s="4">
+        <v>5</v>
+      </c>
+      <c r="C64" s="6">
+        <v>10</v>
+      </c>
+      <c r="D64" s="8">
+        <v>19</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1">
+        <v>65</v>
+      </c>
+      <c r="B65" s="4">
+        <v>5</v>
+      </c>
+      <c r="C65" s="6">
+        <v>10</v>
+      </c>
+      <c r="D65" s="8">
+        <v>20</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1">
+        <v>66</v>
+      </c>
+      <c r="B66" s="4">
+        <v>5</v>
+      </c>
+      <c r="C66" s="6">
+        <v>10</v>
+      </c>
+      <c r="D66" s="8">
+        <v>21</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1">
+        <v>67</v>
+      </c>
+      <c r="B67" s="4">
+        <v>5</v>
+      </c>
+      <c r="C67" s="6">
+        <v>9</v>
+      </c>
+      <c r="D67" s="8">
+        <v>22</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1">
+        <v>68</v>
+      </c>
+      <c r="B68" s="4">
+        <v>5</v>
+      </c>
+      <c r="C68" s="6">
+        <v>9</v>
+      </c>
+      <c r="D68" s="8">
+        <v>23</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1">
+        <v>69</v>
+      </c>
+      <c r="B69" s="4">
+        <v>5</v>
+      </c>
+      <c r="C69" s="6">
+        <v>9</v>
+      </c>
+      <c r="D69" s="8">
+        <v>24</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1">
+        <v>70</v>
+      </c>
+      <c r="B70" s="4">
+        <v>5</v>
+      </c>
+      <c r="C70" s="6">
+        <v>9</v>
+      </c>
+      <c r="D70" s="8">
+        <v>25</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F70" s="1">
+        <v>1</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1">
+        <v>71</v>
+      </c>
+      <c r="B71" s="4">
+        <v>5</v>
+      </c>
+      <c r="C71" s="6">
+        <v>9</v>
+      </c>
+      <c r="D71" s="8">
+        <v>26</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="1">
+        <v>72</v>
+      </c>
+      <c r="B72" s="4">
+        <v>5</v>
+      </c>
+      <c r="C72" s="6">
+        <v>9</v>
+      </c>
+      <c r="D72" s="8">
+        <v>27</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="1">
+        <v>73</v>
+      </c>
+      <c r="B73" s="4">
+        <v>4</v>
+      </c>
+      <c r="C73" s="6">
+        <v>4</v>
+      </c>
+      <c r="D73" s="8">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1">
+        <v>74</v>
+      </c>
+      <c r="B74" s="4">
+        <v>4</v>
+      </c>
+      <c r="C74" s="6">
+        <v>4</v>
+      </c>
+      <c r="D74" s="8">
+        <v>2</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F74" s="1">
+        <v>2</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="1">
+        <v>75</v>
+      </c>
+      <c r="B75" s="4">
+        <v>4</v>
+      </c>
+      <c r="C75" s="6">
+        <v>4</v>
+      </c>
+      <c r="D75" s="8">
+        <v>3</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F75" s="1">
+        <v>2</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1">
+        <v>76</v>
+      </c>
+      <c r="B76" s="4">
+        <v>4</v>
+      </c>
+      <c r="C76" s="6">
+        <v>5</v>
+      </c>
+      <c r="D76" s="8">
+        <v>4</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1">
+        <v>2</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1">
+        <v>77</v>
+      </c>
+      <c r="B77" s="4">
+        <v>4</v>
+      </c>
+      <c r="C77" s="6">
+        <v>5</v>
+      </c>
+      <c r="D77" s="8">
+        <v>5</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1">
+        <v>2</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1">
+        <v>78</v>
+      </c>
+      <c r="B78" s="4">
+        <v>4</v>
+      </c>
+      <c r="C78" s="6">
+        <v>5</v>
+      </c>
+      <c r="D78" s="8">
+        <v>6</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1">
+        <v>2</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="1">
+        <v>79</v>
+      </c>
+      <c r="B79" s="4">
+        <v>4</v>
+      </c>
+      <c r="C79" s="6">
+        <v>6</v>
+      </c>
+      <c r="D79" s="8">
+        <v>7</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F79" s="1">
+        <v>2</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="1">
+        <v>80</v>
+      </c>
+      <c r="B80" s="4">
+        <v>4</v>
+      </c>
+      <c r="C80" s="6">
+        <v>6</v>
+      </c>
+      <c r="D80" s="8">
+        <v>8</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1">
+        <v>2</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
+      <c r="A81" s="1">
+        <v>81</v>
+      </c>
+      <c r="B81" s="4">
+        <v>4</v>
+      </c>
+      <c r="C81" s="6">
+        <v>6</v>
+      </c>
+      <c r="D81" s="8">
+        <v>9</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F81" s="1">
+        <v>2</v>
+      </c>
+      <c r="G81" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H81" s="1">
+        <v>1</v>
+      </c>
+      <c r="K81" s="1">
+        <v>1</v>
+      </c>
+      <c r="L81" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M81">
+        <v>15</v>
+      </c>
+      <c r="N81">
+        <v>1</v>
+      </c>
+      <c r="O81" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>88</v>
+      </c>
+      <c r="R81" s="1">
+        <v>1</v>
+      </c>
+      <c r="S81" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
+      <c r="A82" s="1">
+        <v>82</v>
+      </c>
+      <c r="B82" s="4">
+        <v>6</v>
+      </c>
+      <c r="C82" s="6">
+        <v>11</v>
+      </c>
+      <c r="D82" s="8">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" s="1">
+        <v>3</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H82" s="1">
+        <v>1</v>
+      </c>
+      <c r="K82" s="1">
+        <v>2</v>
+      </c>
+      <c r="L82" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M82">
+        <v>15</v>
+      </c>
+      <c r="N82">
+        <v>2</v>
+      </c>
+      <c r="O82" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>89</v>
+      </c>
+      <c r="R82" s="1">
+        <v>2</v>
+      </c>
+      <c r="S82" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
+      <c r="A83" s="1">
+        <v>83</v>
+      </c>
+      <c r="B83" s="4">
+        <v>6</v>
+      </c>
+      <c r="C83" s="6">
+        <v>11</v>
+      </c>
+      <c r="D83" s="8">
+        <v>2</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1">
+        <v>3</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H83" s="1">
+        <v>1</v>
+      </c>
+      <c r="K83" s="1">
+        <v>3</v>
+      </c>
+      <c r="L83" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M83">
+        <v>15</v>
+      </c>
+      <c r="N83">
+        <v>3</v>
+      </c>
+      <c r="O83" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>87</v>
+      </c>
+      <c r="R83" s="1">
+        <v>3</v>
+      </c>
+      <c r="S83" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19">
+      <c r="A84" s="1">
+        <v>84</v>
+      </c>
+      <c r="B84" s="4">
+        <v>6</v>
+      </c>
+      <c r="C84" s="6">
+        <v>11</v>
+      </c>
+      <c r="D84" s="8">
+        <v>3</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>3</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H84" s="1">
+        <v>1</v>
+      </c>
+      <c r="K84" s="1">
+        <v>4</v>
+      </c>
+      <c r="L84" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84">
+        <v>21</v>
+      </c>
+      <c r="N84">
+        <v>4</v>
+      </c>
+      <c r="O84" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>90</v>
+      </c>
+      <c r="R84" s="1">
+        <v>4</v>
+      </c>
+      <c r="S84" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
+      <c r="A85" s="1">
+        <v>85</v>
+      </c>
+      <c r="B85" s="4">
+        <v>6</v>
+      </c>
+      <c r="C85" s="6">
+        <v>11</v>
+      </c>
+      <c r="D85" s="8">
+        <v>4</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1">
+        <v>3</v>
+      </c>
+      <c r="G85" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H85" s="1">
+        <v>1</v>
+      </c>
+      <c r="K85" s="1">
+        <v>5</v>
+      </c>
+      <c r="L85" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M85">
+        <v>21</v>
+      </c>
+      <c r="N85">
+        <v>5</v>
+      </c>
+      <c r="O85" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>91</v>
+      </c>
+      <c r="R85" s="1">
+        <v>5</v>
+      </c>
+      <c r="S85" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
+      <c r="A86" s="1">
+        <v>86</v>
+      </c>
+      <c r="B86" s="4">
+        <v>6</v>
+      </c>
+      <c r="C86" s="6">
+        <v>15</v>
+      </c>
+      <c r="D86" s="8">
+        <v>5</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F86" s="1">
+        <v>3</v>
+      </c>
+      <c r="G86" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H86" s="1">
+        <v>1</v>
+      </c>
+      <c r="K86" s="1">
+        <v>6</v>
+      </c>
+      <c r="L86" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M86">
+        <v>21</v>
+      </c>
+      <c r="N86">
+        <v>6</v>
+      </c>
+      <c r="O86" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>92</v>
+      </c>
+      <c r="R86" s="1">
+        <v>6</v>
+      </c>
+      <c r="S86" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19">
+      <c r="A87" s="1">
+        <v>87</v>
+      </c>
+      <c r="B87" s="4">
+        <v>6</v>
+      </c>
+      <c r="C87" s="6">
+        <v>15</v>
+      </c>
+      <c r="D87" s="8">
+        <v>6</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1">
+        <v>3</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H87" s="1">
+        <v>1</v>
+      </c>
+      <c r="K87" s="1">
+        <v>7</v>
+      </c>
+      <c r="L87" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M87">
+        <v>18</v>
+      </c>
+      <c r="N87">
+        <v>7</v>
+      </c>
+      <c r="O87" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>93</v>
+      </c>
+      <c r="R87" s="1">
+        <v>7</v>
+      </c>
+      <c r="S87" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19">
+      <c r="A88" s="1">
+        <v>88</v>
+      </c>
+      <c r="B88" s="4">
+        <v>6</v>
+      </c>
+      <c r="C88" s="6">
+        <v>15</v>
+      </c>
+      <c r="D88" s="8">
+        <v>7</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1">
+        <v>3</v>
+      </c>
+      <c r="G88" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H88" s="1">
+        <v>1</v>
+      </c>
+      <c r="K88" s="1">
+        <v>8</v>
+      </c>
+      <c r="L88" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M88">
+        <v>18</v>
+      </c>
+      <c r="N88">
+        <v>8</v>
+      </c>
+      <c r="O88" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>8</v>
+      </c>
+      <c r="R88" s="1">
+        <v>8</v>
+      </c>
+      <c r="S88" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19">
+      <c r="A89" s="1">
+        <v>89</v>
+      </c>
+      <c r="B89" s="4">
+        <v>6</v>
+      </c>
+      <c r="C89" s="6">
+        <v>15</v>
+      </c>
+      <c r="D89" s="8">
+        <v>8</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1">
+        <v>3</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H89" s="1">
+        <v>1</v>
+      </c>
+      <c r="K89" s="1">
+        <v>9</v>
+      </c>
+      <c r="L89" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M89">
+        <v>18</v>
+      </c>
+      <c r="N89">
+        <v>9</v>
+      </c>
+      <c r="O89" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>8</v>
+      </c>
+      <c r="R89" s="1">
+        <v>9</v>
+      </c>
+      <c r="S89" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
+      <c r="A90" s="1">
+        <v>90</v>
+      </c>
+      <c r="B90" s="4">
+        <v>6</v>
+      </c>
+      <c r="C90" s="6">
+        <v>15</v>
+      </c>
+      <c r="D90" s="8">
+        <v>9</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F90" s="1">
+        <v>3</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H90" s="1">
+        <v>1</v>
+      </c>
+      <c r="M90">
+        <v>18</v>
+      </c>
+      <c r="N90">
+        <v>10</v>
+      </c>
+      <c r="O90" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
+      <c r="M91">
+        <v>16</v>
+      </c>
+      <c r="N91">
+        <v>11</v>
+      </c>
+      <c r="O91" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
+      <c r="M92">
+        <v>18</v>
+      </c>
+      <c r="N92">
+        <v>12</v>
+      </c>
+      <c r="O92" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
+      <c r="M93">
+        <v>12</v>
+      </c>
+      <c r="N93">
+        <v>13</v>
+      </c>
+      <c r="O93" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19">
+      <c r="M94">
+        <v>15</v>
+      </c>
+      <c r="N94">
+        <v>14</v>
+      </c>
+      <c r="O94" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19">
+      <c r="M95">
+        <v>20</v>
+      </c>
+      <c r="N95">
+        <v>15</v>
+      </c>
+      <c r="O95" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19">
+      <c r="M96">
+        <v>18</v>
+      </c>
+      <c r="N96">
+        <v>16</v>
+      </c>
+      <c r="O96" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G28:G29" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2415,7 +5620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>